<commit_message>
A tiny tidy up
</commit_message>
<xml_diff>
--- a/Experiment/Experiment's Timetable.xlsx
+++ b/Experiment/Experiment's Timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\Documents\Studium\Master\Trient\Uni Trient\Multisensory Interactive Systems\Final-MIS-Project\Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Final-MIS-Project\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CF124F-FBA2-4224-A6A2-E6212DD5E5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27B3AC1-3342-4B6A-9356-381D5E94120F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>No.</t>
   </si>
@@ -43,15 +43,6 @@
   </si>
   <si>
     <t>Sam</t>
-  </si>
-  <si>
-    <t>Enrica</t>
-  </si>
-  <si>
-    <t>Lucia</t>
-  </si>
-  <si>
-    <t>Asia</t>
   </si>
   <si>
     <t>Prince</t>
@@ -221,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -280,9 +271,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -568,28 +560,28 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.8984375" customWidth="1"/>
-    <col min="2" max="2" width="19.296875" customWidth="1"/>
-    <col min="3" max="3" width="10.8984375" customWidth="1"/>
-    <col min="4" max="4" width="17.296875" customWidth="1"/>
-    <col min="5" max="5" width="16.09765625" customWidth="1"/>
-    <col min="6" max="6" width="16.3984375" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>1</v>
@@ -601,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -609,233 +601,212 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="F3" s="10">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="11">
-        <v>0.64583333333333337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="13">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="13">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="13">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16">
+        <v>0.625</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="17">
-        <v>0.64583333333333337</v>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="13">
+        <v>0.6875</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="17">
+        <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="13">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E10" s="1"/>
+      <c r="B10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="23">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="13">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E11" s="1"/>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="17">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="13">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="E12" s="1"/>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="17">
+        <v>0.6875</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="17">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="13">
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="F14" s="10">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>13</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="11">
+        <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="17">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="26.9" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="17">
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="17">
-        <v>0.52083333333333337</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Removed the cancelled participants
</commit_message>
<xml_diff>
--- a/Experiment/Experiment's Timetable.xlsx
+++ b/Experiment/Experiment's Timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e046d29d2472528d/Documenti/GitHub/Final-MIS-Project/Experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Final-MIS-Project\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{A32DC70E-DAEA-4441-9661-C5B01FD967D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85F50BE1-4433-4252-9035-A12F7AE2AF1B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB33F9A-51D4-4E5D-A6E1-BF2CB91A7FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1950" windowWidth="28800" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>No.</t>
   </si>
@@ -43,15 +43,6 @@
   </si>
   <si>
     <t>Sam</t>
-  </si>
-  <si>
-    <t>Enrica</t>
-  </si>
-  <si>
-    <t>Lucia</t>
-  </si>
-  <si>
-    <t>Asia</t>
   </si>
   <si>
     <t>Prince</t>
@@ -224,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -283,6 +274,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,17 +562,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
@@ -589,10 +583,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>1</v>
@@ -616,26 +610,28 @@
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="F3" s="10">
-        <v>0.625</v>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="11">
-        <v>0.64583333333333337</v>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.52083333333333337</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -643,217 +639,191 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E5" s="24"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E6" s="24"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="E7" s="24"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="17">
-        <v>0.64583333333333337</v>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.6875</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="17">
-        <v>0.66666666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="17">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="17">
         <v>0.6875</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="13">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E12" s="1"/>
+      <c r="C12" s="22"/>
+      <c r="E12" s="23">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="13">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="E13" s="23">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="13">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="F14" s="10">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
-        <v>11</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="16">
-        <v>0.625</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="11">
+        <v>0.64583333333333337</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="13">
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
-        <v>13</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="23">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
-        <v>14</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="23">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
re-add lost participant (Anna)
</commit_message>
<xml_diff>
--- a/Experiment/Experiment's Timetable.xlsx
+++ b/Experiment/Experiment's Timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Final-MIS-Project\Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\Documents\Studium\Master\Trient\Uni Trient\Multisensory Interactive Systems\Final-MIS-Project\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB33F9A-51D4-4E5D-A6E1-BF2CB91A7FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184D6ADD-4764-447F-AB64-78AC045351AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>No.</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Gianmarco</t>
+  </si>
+  <si>
+    <t>Anna</t>
   </si>
 </sst>
 </file>
@@ -279,7 +282,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -565,20 +568,20 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.8984375" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.8984375" customWidth="1"/>
+    <col min="2" max="2" width="28.296875" customWidth="1"/>
+    <col min="3" max="3" width="11.09765625" customWidth="1"/>
+    <col min="4" max="4" width="17.296875" customWidth="1"/>
+    <col min="5" max="5" width="16.09765625" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -598,7 +601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -606,7 +609,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -620,7 +623,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -634,7 +637,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -650,7 +653,7 @@
       <c r="E5" s="24"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -666,7 +669,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -682,7 +685,7 @@
       <c r="E7" s="24"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -697,132 +700,141 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="17">
-        <v>0.64583333333333337</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="17">
-        <v>0.66666666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1"/>
       <c r="E11" s="17">
-        <v>0.6875</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="18.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="E12" s="23">
-        <v>0.70833333333333337</v>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="17">
+        <v>0.6875</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>20</v>
+      <c r="B13" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="C13" s="22"/>
       <c r="E13" s="23">
-        <v>0.72916666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="F14" s="10">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="E14" s="23">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="11">
-        <v>0.64583333333333337</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="F15" s="10">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="11">
+        <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Separate first mode for Males and Females
</commit_message>
<xml_diff>
--- a/Experiment/Experiment's Timetable.xlsx
+++ b/Experiment/Experiment's Timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\Documents\Studium\Master\Trient\Uni Trient\Multisensory Interactive Systems\Final-MIS-Project\Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Final-MIS-Project\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184D6ADD-4764-447F-AB64-78AC045351AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D41BBA8-F3A9-4E16-964D-D74679DCD168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>No.</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Luca</t>
   </si>
   <si>
-    <t>First Mode</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -91,6 +88,12 @@
   </si>
   <si>
     <t>Anna</t>
+  </si>
+  <si>
+    <t>First Mode (Females)</t>
+  </si>
+  <si>
+    <t>First Mode (Males)</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -565,23 +568,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.8984375" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.8984375" customWidth="1"/>
-    <col min="2" max="2" width="28.296875" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" customWidth="1"/>
-    <col min="4" max="4" width="17.296875" customWidth="1"/>
-    <col min="5" max="5" width="16.09765625" customWidth="1"/>
-    <col min="6" max="6" width="16.3984375" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -589,27 +593,31 @@
         <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -617,27 +625,29 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="13">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="13">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="13">
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -645,15 +655,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="13">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="24"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -661,31 +672,33 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="13">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="13">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="24"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="16">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="16">
         <v>0.625</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="24"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -693,28 +706,32 @@
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="13">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="13">
         <v>0.6875</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="17">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="17">
         <v>0.52083333333333337</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -722,68 +739,83 @@
         <v>6</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="17">
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="17">
         <v>0.64583333333333337</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="17">
+      <c r="D11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" ht="18.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="17">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="17">
         <v>0.6875</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="E13" s="23">
+        <v>17</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="F13" s="23">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="M13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="1"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>12</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="E14" s="23">
+      <c r="D14" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="23">
         <v>0.72916666666666663</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -791,11 +823,14 @@
         <v>5</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="F15" s="10">
+      <c r="D15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="10">
         <v>0.625</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -803,38 +838,41 @@
         <v>4</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="11">
+      <c r="F16" s="1"/>
+      <c r="G16" s="11">
         <v>0.64583333333333337</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
add participant (Sveta), move Isabel
</commit_message>
<xml_diff>
--- a/Experiment/Experiment's Timetable.xlsx
+++ b/Experiment/Experiment's Timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Final-MIS-Project\Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\Documents\Studium\Master\Trient\Uni Trient\Multisensory Interactive Systems\Final-MIS-Project\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D41BBA8-F3A9-4E16-964D-D74679DCD168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10933F89-EC25-4F5F-8A3A-CC5CB751B202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>No.</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>First Mode (Males)</t>
+  </si>
+  <si>
+    <t>Sveta (English only)</t>
   </si>
 </sst>
 </file>
@@ -285,7 +288,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -571,21 +574,21 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.8984375" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.8984375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.09765625" customWidth="1"/>
+    <col min="4" max="4" width="17.3984375" customWidth="1"/>
+    <col min="5" max="5" width="17.296875" customWidth="1"/>
+    <col min="6" max="6" width="16.09765625" customWidth="1"/>
+    <col min="7" max="7" width="16.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="25.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -608,7 +611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -617,7 +620,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -632,7 +635,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -647,7 +650,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -664,7 +667,7 @@
       <c r="F5" s="24"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -681,7 +684,7 @@
       <c r="F6" s="24"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -698,7 +701,7 @@
       <c r="F7" s="24"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -714,7 +717,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -731,7 +734,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -748,7 +751,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -765,7 +768,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="18.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -782,12 +785,12 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>14</v>
@@ -799,7 +802,7 @@
       <c r="G13" s="1"/>
       <c r="N13" s="9"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -815,7 +818,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -830,7 +833,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -847,32 +850,42 @@
         <v>0.64583333333333337</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>20</v>
       </c>

</xml_diff>